<commit_message>
VyTrack tests are WIP
</commit_message>
<xml_diff>
--- a/VyTrackQa2Users.xlsx
+++ b/VyTrackQa2Users.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mustafacetinkaya/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52FC1A35-5BAE-8C4A-B6B1-27D635DA2AE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FD87FE9-8F61-D646-82B6-082F10EDC382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16000" xr2:uid="{B51DDFA4-018A-C44D-AE61-28C3EC3E0526}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
   <si>
     <t>FirstName</t>
   </si>
@@ -55,18 +55,6 @@
     <t>UserUser123</t>
   </si>
   <si>
-    <t>UserUser124</t>
-  </si>
-  <si>
-    <t>UserUser125</t>
-  </si>
-  <si>
-    <t>UserUser126</t>
-  </si>
-  <si>
-    <t>UserUser127</t>
-  </si>
-  <si>
     <t>user1</t>
   </si>
   <si>
@@ -122,12 +110,19 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>FAILED</t>
+  </si>
+  <si>
+    <t>PASSES</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -507,13 +502,13 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="161" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" customWidth="1"/>
-    <col min="2" max="2" width="14.5" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="17.33203125"/>
+    <col min="2" max="2" customWidth="true" width="14.5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -535,104 +530,104 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>